<commit_message>
New data files are files messing with growth rate.
</commit_message>
<xml_diff>
--- a/processed_data/head_growth_wide.xlsx
+++ b/processed_data/head_growth_wide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmg31\Box\Katy\Research\Experiments\Pteronarcys_Sulfate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmg31\Box\Katy\Research\experiments\sulfate\pteronarcys\processed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08C8C09-70DE-4FD8-99B0-F318570FA118}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB34303-F4AB-4855-AD66-226605E44ABC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0B05E6ED-A467-4E33-B61F-B6C80C7EC048}"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="12900" windowHeight="12360" xr2:uid="{0B05E6ED-A467-4E33-B61F-B6C80C7EC048}"/>
   </bookViews>
   <sheets>
     <sheet name="Ptery_Sulfate Growth" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="364">
   <si>
     <t>TANK</t>
   </si>
@@ -1126,6 +1126,9 @@
   </si>
   <si>
     <t>08A</t>
+  </si>
+  <si>
+    <t>38D1</t>
   </si>
 </sst>
 </file>
@@ -11617,8 +11620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{348700C6-BE42-4EFE-B99F-31CA8EAF49DC}">
   <dimension ref="A1:P361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="P333" sqref="P333"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12104,7 +12107,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>363</v>
       </c>
       <c r="E11" s="2">
         <v>1.7555555555555555</v>
@@ -15817,6 +15820,12 @@
       </c>
       <c r="K100">
         <v>1.6888888888888889</v>
+      </c>
+      <c r="L100">
+        <v>1.6888888888888889</v>
+      </c>
+      <c r="M100">
+        <v>1.711111111111111</v>
       </c>
       <c r="N100">
         <f>VLOOKUP(D100,'[1]Ptery_Sulfate Head Measurements'!$E$2637:$H$2877,4,FALSE)</f>

</xml_diff>